<commit_message>
Made code more clean
</commit_message>
<xml_diff>
--- a/Graphics.XLSX
+++ b/Graphics.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\35498\source\repos\OlegZuev\KnapsackProblem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F9E58D-A84D-4CEC-9F18-D8757583E890}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2214EDA-0ABE-41DB-BA8B-F33FC146E07C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="870" yWindow="300" windowWidth="27420" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,6 +86,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -344,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -389,6 +392,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -3150,7 +3155,7 @@
             <c:numRef>
               <c:f>Iter!$B$32:$M$32</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -3393,7 +3398,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -9120,8 +9125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V84" sqref="V84"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10255,40 +10260,40 @@
       <c r="A32" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="20">
+      <c r="B32" s="30">
         <v>0</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="31">
         <v>3.1E-2</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="31">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="31">
         <v>2.92E-2</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F32" s="31">
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="31">
         <v>2.5899999999999999E-2</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="31">
         <v>2.1700000000000001E-2</v>
       </c>
-      <c r="I32" s="9">
+      <c r="I32" s="31">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="J32" s="9">
+      <c r="J32" s="31">
         <v>2.1600000000000001E-2</v>
       </c>
-      <c r="K32" s="9">
+      <c r="K32" s="31">
         <v>1.9699999999999999E-2</v>
       </c>
-      <c r="L32" s="9">
+      <c r="L32" s="31">
         <v>1.9199999999999998E-2</v>
       </c>
-      <c r="M32" s="9">
+      <c r="M32" s="31">
         <v>1.7299999999999999E-2</v>
       </c>
       <c r="N32" s="8"/>

</xml_diff>